<commit_message>
Add annotations package contains: 'FrameworkAnnotation' class, update @Test with annotations used in 'FrameworkAnnotations'
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F159C1E-9A24-4840-B11A-C00A0638A6E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844740AA-4753-4E2E-BC5C-E2F6D9B0CDC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -506,7 +506,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +543,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
@@ -577,7 +577,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
@@ -597,7 +597,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +642,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>23</v>
@@ -668,7 +668,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>24</v>
@@ -772,7 +772,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Add 'DecodeUtils' class with getDecodedString method, and update 'OrangeHRMLoginPage' class with getDecodedString method
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844740AA-4753-4E2E-BC5C-E2F6D9B0CDC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B579B9-CFCE-4274-B4B7-9C8933DBC0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="35">
   <si>
     <t>testname</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>69.0</t>
+  </si>
+  <si>
+    <t>YWRtaTEyMw==</t>
   </si>
 </sst>
 </file>
@@ -597,7 +600,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +657,7 @@
         <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>19</v>
@@ -680,7 +683,7 @@
         <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>20</v>
@@ -706,7 +709,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Update config.properties file, and create DriverFactory class
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B579B9-CFCE-4274-B4B7-9C8933DBC0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4712EEF6-FF21-4AE1-8381-E449F1C7F954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -114,13 +114,13 @@
     <t>79.0.3945.117</t>
   </si>
   <si>
-    <t>88.0.4324.96</t>
-  </si>
-  <si>
-    <t>69.0</t>
-  </si>
-  <si>
     <t>YWRtaTEyMw==</t>
+  </si>
+  <si>
+    <t>92.0.1</t>
+  </si>
+  <si>
+    <t>94.0.4606.61</t>
   </si>
 </sst>
 </file>
@@ -509,7 +509,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,14 +600,14 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.28515625" customWidth="1"/>
     <col min="2" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" customWidth="1"/>
     <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
@@ -651,13 +651,13 @@
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>19</v>
@@ -683,7 +683,7 @@
         <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>20</v>
@@ -703,13 +703,13 @@
         <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>17</v>
@@ -807,7 +807,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Add docker-compose.yaml file for docker container, docker images (selenium/hub, selenium-firefox, selenium-chrome)
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4712EEF6-FF21-4AE1-8381-E449F1C7F954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922F392D-6728-42C1-9A61-63E2CCCC1101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -600,7 +600,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,7 +801,7 @@
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>23</v>
@@ -827,7 +827,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>24</v>

</xml_diff>